<commit_message>
- improve the search - export
</commit_message>
<xml_diff>
--- a/in.xlsx
+++ b/in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/product/eng_pro/word_family/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2682D56B-634C-2A4C-88BD-2FD76677EA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671A0786-7012-7243-B9B9-67C07898BCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{F382C1B7-36CD-044F-B3F5-21E1AF52B46D}"/>
   </bookViews>
@@ -25,18 +25,12 @@
     <t>word</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
     <t>grade</t>
   </si>
   <si>
     <t>unit</t>
   </si>
   <si>
-    <t>Section</t>
-  </si>
-  <si>
     <t>test_point</t>
   </si>
   <si>
@@ -251,6 +245,12 @@
   </si>
   <si>
     <t>People speak Chinese in _____.</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>reference</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,8 +1105,8 @@
     <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1115,1434 +1115,1435 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" t="s">
-        <v>32</v>
-      </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I32" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E40" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I41" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E46" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G48" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E49" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F49" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G51" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E52" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C53" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E53" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G53" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E54" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I54" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E55" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F55" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G55" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I55" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E56" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F56" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G56" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I56" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E57" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I57" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E58" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G58" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E59" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F59" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G59" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I59" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E60" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F60" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G60" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I60" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C61" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E61" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F61" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G61" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E62" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G62" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I62" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>